<commit_message>
Update square notation mei mapping files
</commit_message>
<xml_diff>
--- a/resources/4_mei_encoding/SQUAREnotation-NClevel.xlsx
+++ b/resources/4_mei_encoding/SQUAREnotation-NClevel.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2" conformance="strict">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10119"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
   <workbookPr dateCompatibility="0" defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mthomae/Downloads/OMR_Portuguese_Sources/resources/4_mei_encoding/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mthomae/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{B29E5D9B-CE43-0041-B14B-EEAD48E2BDC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{B6F2A01D-06D4-AD43-B42C-A1917BE98F57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="13640" yWindow="3520" windowWidth="33220" windowHeight="23520" xr2:uid="{0394C6CE-5AF9-CF4B-B63B-6BC72F9E9ED6}"/>
   </bookViews>
@@ -157,7 +157,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="98" uniqueCount="84">
+<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="208" uniqueCount="111">
   <si>
     <t>imagePath</t>
   </si>
@@ -329,9 +329,6 @@
 &lt;/neume&gt;</t>
   </si>
   <si>
-    <t>[1, 1]</t>
-  </si>
-  <si>
     <t>neume.lenguetaup</t>
   </si>
   <si>
@@ -446,12 +443,96 @@
   <si>
     <t>Obliqua1 middle</t>
   </si>
+  <si>
+    <t>[]</t>
+  </si>
+  <si>
+    <t>Flat</t>
+  </si>
+  <si>
+    <t>accid.flat</t>
+  </si>
+  <si>
+    <t>&lt;accid accid="f"/&gt;</t>
+  </si>
+  <si>
+    <t>Custos</t>
+  </si>
+  <si>
+    <t>custos</t>
+  </si>
+  <si>
+    <t>&lt;custos/&gt;</t>
+  </si>
+  <si>
+    <t>Divisio</t>
+  </si>
+  <si>
+    <t>divisio</t>
+  </si>
+  <si>
+    <t>&lt;divLine/&gt;</t>
+  </si>
+  <si>
+    <t>Clivis</t>
+  </si>
+  <si>
+    <t>neume.clivis</t>
+  </si>
+  <si>
+    <t>[1,1]</t>
+  </si>
+  <si>
+    <t>&lt;neume&gt;</t>
+  </si>
+  <si>
+    <t>    &lt;nc/&gt;</t>
+  </si>
+  <si>
+    <t>    &lt;nc intm="-1S"/&gt;</t>
+  </si>
+  <si>
+    <t>&lt;/neume&gt;</t>
+  </si>
+  <si>
+    <t>Podatus</t>
+  </si>
+  <si>
+    <t>neume.podatus</t>
+  </si>
+  <si>
+    <t>    &lt;nc intm="1S"/&gt;</t>
+  </si>
+  <si>
+    <t>    &lt;nc ligated="true"/&gt;</t>
+  </si>
+  <si>
+    <t>    &lt;nc intm="-1S" ligated="true"/&gt;</t>
+  </si>
+  <si>
+    <t>Plica down</t>
+  </si>
+  <si>
+    <t>neume.twolegsdown</t>
+  </si>
+  <si>
+    <t>&lt;neume type="twolegsdown"&gt;</t>
+  </si>
+  <si>
+    <t>    &lt;nc intm="0S"/&gt;</t>
+  </si>
+  <si>
+    <t>Torculus11</t>
+  </si>
+  <si>
+    <t>neume.torculus11</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="21" x14ac:knownFonts="1">
+  <fonts count="23" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -603,6 +684,19 @@
       <color theme="1"/>
       <name val="Aptos Narrow"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Helvetica Neue"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Helvetica Neue"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="33">
@@ -946,7 +1040,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -954,6 +1048,19 @@
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1448,13 +1555,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A001BD3-14A6-E347-AC0D-A7B160A0B128}">
-  <dimension ref="A1:K15"/>
+  <dimension ref="A1:K39"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="E13" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C6" sqref="C6"/>
+      <selection pane="bottomRight" activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1465,7 +1572,7 @@
     <col min="4" max="4" width="4.6640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="32" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="19.83203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.83203125" style="9" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="29.33203125" customWidth="1"/>
     <col min="9" max="9" width="6.5" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="4.1640625" bestFit="1" customWidth="1"/>
@@ -1491,7 +1598,7 @@
       <c r="F1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="9" t="s">
         <v>6</v>
       </c>
       <c r="H1" t="s">
@@ -1518,22 +1625,22 @@
         <v>11</v>
       </c>
       <c r="D2" t="s">
+        <v>56</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>57</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>58</v>
       </c>
       <c r="F2" t="s">
         <v>12</v>
       </c>
-      <c r="G2">
+      <c r="G2" s="9">
         <v>1</v>
       </c>
       <c r="H2" s="1" t="s">
         <v>13</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="49" customHeight="1" x14ac:dyDescent="0.2">
@@ -1550,19 +1657,19 @@
         <v>27</v>
       </c>
       <c r="E3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F3" t="s">
         <v>18</v>
       </c>
-      <c r="G3">
+      <c r="G3" s="9">
         <v>1</v>
       </c>
       <c r="H3" s="1" t="s">
         <v>14</v>
       </c>
       <c r="K3" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="102" x14ac:dyDescent="0.2">
@@ -1576,22 +1683,22 @@
         <v>19</v>
       </c>
       <c r="D4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F4" t="s">
         <v>20</v>
       </c>
-      <c r="G4">
+      <c r="G4" s="9">
         <v>1</v>
       </c>
       <c r="H4" s="1" t="s">
         <v>24</v>
       </c>
       <c r="K4" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="66" customHeight="1" x14ac:dyDescent="0.2">
@@ -1602,25 +1709,25 @@
         <v>#VALUE!</v>
       </c>
       <c r="C5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D5">
         <v>355</v>
       </c>
       <c r="E5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F5" t="s">
-        <v>51</v>
-      </c>
-      <c r="G5" t="s">
-        <v>46</v>
+        <v>50</v>
+      </c>
+      <c r="G5" s="9">
+        <v>1</v>
       </c>
       <c r="H5" s="1" t="s">
         <v>42</v>
       </c>
       <c r="K5" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="68" customHeight="1" x14ac:dyDescent="0.2">
@@ -1631,25 +1738,25 @@
         <v>#VALUE!</v>
       </c>
       <c r="C6" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D6">
         <v>348</v>
       </c>
       <c r="E6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F6" t="s">
-        <v>50</v>
-      </c>
-      <c r="G6" t="s">
-        <v>46</v>
+        <v>49</v>
+      </c>
+      <c r="G6" s="9">
+        <v>1</v>
       </c>
       <c r="H6" s="1" t="s">
         <v>43</v>
       </c>
       <c r="K6" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="60" customHeight="1" x14ac:dyDescent="0.2">
@@ -1660,25 +1767,25 @@
         <v>#VALUE!</v>
       </c>
       <c r="C7" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D7">
         <v>131</v>
       </c>
       <c r="E7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F7" t="s">
-        <v>49</v>
-      </c>
-      <c r="G7" t="s">
-        <v>46</v>
+        <v>48</v>
+      </c>
+      <c r="G7" s="9">
+        <v>1</v>
       </c>
       <c r="H7" s="1" t="s">
         <v>44</v>
       </c>
       <c r="K7" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="50" customHeight="1" x14ac:dyDescent="0.2">
@@ -1695,19 +1802,19 @@
         <v>348</v>
       </c>
       <c r="E8" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F8" t="s">
         <v>16</v>
       </c>
-      <c r="G8">
+      <c r="G8" s="9">
         <v>1</v>
       </c>
       <c r="H8" s="1" t="s">
         <v>40</v>
       </c>
       <c r="K8" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="63" customHeight="1" x14ac:dyDescent="0.2">
@@ -1718,25 +1825,25 @@
         <v>#VALUE!</v>
       </c>
       <c r="C9" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D9" t="s">
+        <v>65</v>
+      </c>
+      <c r="E9" t="s">
         <v>66</v>
       </c>
-      <c r="E9" t="s">
-        <v>67</v>
-      </c>
       <c r="F9" t="s">
-        <v>48</v>
-      </c>
-      <c r="G9">
+        <v>47</v>
+      </c>
+      <c r="G9" s="9">
         <v>1</v>
       </c>
       <c r="H9" s="1" t="s">
         <v>39</v>
       </c>
       <c r="K9" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="68" x14ac:dyDescent="0.2">
@@ -1747,25 +1854,25 @@
         <v>#VALUE!</v>
       </c>
       <c r="C10" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D10">
         <v>348</v>
       </c>
       <c r="E10" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F10" t="s">
-        <v>47</v>
-      </c>
-      <c r="G10">
+        <v>46</v>
+      </c>
+      <c r="G10" s="9">
         <v>1</v>
       </c>
       <c r="H10" s="1" t="s">
         <v>45</v>
       </c>
       <c r="K10" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="11" spans="1:11" ht="84" customHeight="1" x14ac:dyDescent="0.2">
@@ -1782,19 +1889,19 @@
         <v>91</v>
       </c>
       <c r="E11" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F11" t="s">
         <v>23</v>
       </c>
-      <c r="G11" t="s">
+      <c r="G11" s="9" t="s">
         <v>21</v>
       </c>
       <c r="H11" s="1" t="s">
         <v>25</v>
       </c>
       <c r="K11" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="12" spans="1:11" ht="84" customHeight="1" x14ac:dyDescent="0.2">
@@ -1811,79 +1918,693 @@
         <v>12</v>
       </c>
       <c r="E12" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F12" t="s">
         <v>38</v>
       </c>
-      <c r="G12" t="s">
+      <c r="G12" s="9" t="s">
         <v>21</v>
       </c>
       <c r="H12" s="1" t="s">
         <v>37</v>
       </c>
       <c r="K12" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="13" spans="1:11" ht="85" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B13" t="e" vm="12">
         <v>#VALUE!</v>
       </c>
       <c r="C13" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D13">
         <v>3</v>
       </c>
       <c r="E13" t="s">
+        <v>71</v>
+      </c>
+      <c r="F13" t="s">
+        <v>53</v>
+      </c>
+      <c r="G13" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="K13" s="3" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A14" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="E14" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="F14" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="F13" t="s">
-        <v>54</v>
-      </c>
-      <c r="G13" t="s">
+      <c r="G14" s="10">
+        <v>1</v>
+      </c>
+      <c r="H14" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="I14" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="J14" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="K14" s="6" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A15" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="E15" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="F15" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="G15" s="10">
+        <v>1</v>
+      </c>
+      <c r="H15" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="I15" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="J15" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="K15" s="6" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A16" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="D16" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="E16" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="F16" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="G16" s="10">
+        <v>1</v>
+      </c>
+      <c r="H16" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="I16" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="J16" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="K16" s="6" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A17" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="D17" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="E17" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="F17" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="G17" s="10">
+        <v>1</v>
+      </c>
+      <c r="H17" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="I17" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="J17" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="K17" s="6" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A18" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="D18" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="E18" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="F18" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="G18" s="10">
+        <v>1</v>
+      </c>
+      <c r="H18" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="I18" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="J18" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="K18" s="6" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A19" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="B19" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="C19" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="D19" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="E19" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="F19" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="G19" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="H19" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="I19" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="J19" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="K19" s="8" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A20" s="7"/>
+      <c r="B20" s="8"/>
+      <c r="C20" s="8"/>
+      <c r="D20" s="8"/>
+      <c r="E20" s="8"/>
+      <c r="F20" s="8"/>
+      <c r="G20" s="11"/>
+      <c r="H20" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="I20" s="8"/>
+      <c r="J20" s="8"/>
+      <c r="K20" s="8"/>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A21" s="7"/>
+      <c r="B21" s="8"/>
+      <c r="C21" s="8"/>
+      <c r="D21" s="8"/>
+      <c r="E21" s="8"/>
+      <c r="F21" s="8"/>
+      <c r="G21" s="11"/>
+      <c r="H21" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="I21" s="8"/>
+      <c r="J21" s="8"/>
+      <c r="K21" s="8"/>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A22" s="7"/>
+      <c r="B22" s="8"/>
+      <c r="C22" s="8"/>
+      <c r="D22" s="8"/>
+      <c r="E22" s="8"/>
+      <c r="F22" s="8"/>
+      <c r="G22" s="11"/>
+      <c r="H22" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="I22" s="8"/>
+      <c r="J22" s="8"/>
+      <c r="K22" s="8"/>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A23" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="B23" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="C23" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="D23" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="E23" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="F23" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="G23" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="H23" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="I23" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="J23" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="K23" s="8" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A24" s="7"/>
+      <c r="B24" s="8"/>
+      <c r="C24" s="8"/>
+      <c r="D24" s="8"/>
+      <c r="E24" s="8"/>
+      <c r="F24" s="8"/>
+      <c r="G24" s="11"/>
+      <c r="H24" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="I24" s="8"/>
+      <c r="J24" s="8"/>
+      <c r="K24" s="8"/>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A25" s="7"/>
+      <c r="B25" s="8"/>
+      <c r="C25" s="8"/>
+      <c r="D25" s="8"/>
+      <c r="E25" s="8"/>
+      <c r="F25" s="8"/>
+      <c r="G25" s="11"/>
+      <c r="H25" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="I25" s="8"/>
+      <c r="J25" s="8"/>
+      <c r="K25" s="8"/>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A26" s="7"/>
+      <c r="B26" s="8"/>
+      <c r="C26" s="8"/>
+      <c r="D26" s="8"/>
+      <c r="E26" s="8"/>
+      <c r="F26" s="8"/>
+      <c r="G26" s="11"/>
+      <c r="H26" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="I26" s="8"/>
+      <c r="J26" s="8"/>
+      <c r="K26" s="8"/>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A27" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="B27" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="C27" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="D27" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="E27" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="F27" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="G27" s="11">
+        <v>1</v>
+      </c>
+      <c r="H27" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="I27" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="J27" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="K27" s="8" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A28" s="7"/>
+      <c r="B28" s="8"/>
+      <c r="C28" s="8"/>
+      <c r="D28" s="8"/>
+      <c r="E28" s="8"/>
+      <c r="F28" s="8"/>
+      <c r="G28" s="11"/>
+      <c r="H28" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="I28" s="8"/>
+      <c r="J28" s="8"/>
+      <c r="K28" s="8"/>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A29" s="7"/>
+      <c r="B29" s="8"/>
+      <c r="C29" s="8"/>
+      <c r="D29" s="8"/>
+      <c r="E29" s="8"/>
+      <c r="F29" s="8"/>
+      <c r="G29" s="11"/>
+      <c r="H29" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="I29" s="8"/>
+      <c r="J29" s="8"/>
+      <c r="K29" s="8"/>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A30" s="7"/>
+      <c r="B30" s="8"/>
+      <c r="C30" s="8"/>
+      <c r="D30" s="8"/>
+      <c r="E30" s="8"/>
+      <c r="F30" s="8"/>
+      <c r="G30" s="11"/>
+      <c r="H30" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="I30" s="8"/>
+      <c r="J30" s="8"/>
+      <c r="K30" s="8"/>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A31" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="B31" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="C31" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="D31" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="E31" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="F31" s="8" t="s">
+        <v>106</v>
+      </c>
+      <c r="G31" s="11">
+        <v>1</v>
+      </c>
+      <c r="H31" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="I31" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="J31" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="K31" s="8" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A32" s="7"/>
+      <c r="B32" s="8"/>
+      <c r="C32" s="8"/>
+      <c r="D32" s="8"/>
+      <c r="E32" s="8"/>
+      <c r="F32" s="8"/>
+      <c r="G32" s="11"/>
+      <c r="H32" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="I32" s="8"/>
+      <c r="J32" s="8"/>
+      <c r="K32" s="8"/>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A33" s="7"/>
+      <c r="B33" s="8"/>
+      <c r="C33" s="8"/>
+      <c r="D33" s="8"/>
+      <c r="E33" s="8"/>
+      <c r="F33" s="8"/>
+      <c r="G33" s="11"/>
+      <c r="H33" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="I33" s="8"/>
+      <c r="J33" s="8"/>
+      <c r="K33" s="8"/>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A34" s="7"/>
+      <c r="B34" s="8"/>
+      <c r="C34" s="8"/>
+      <c r="D34" s="8"/>
+      <c r="E34" s="8"/>
+      <c r="F34" s="8"/>
+      <c r="G34" s="11"/>
+      <c r="H34" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="I34" s="8"/>
+      <c r="J34" s="8"/>
+      <c r="K34" s="8"/>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A35" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="B35" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="C35" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="D35" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="E35" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="F35" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="G35" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="H13" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="K13" s="3" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" ht="17" x14ac:dyDescent="0.2">
-      <c r="C14" t="s">
-        <v>77</v>
-      </c>
-      <c r="F14" t="s">
-        <v>73</v>
-      </c>
-      <c r="G14">
-        <v>1</v>
-      </c>
-      <c r="H14" s="1" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" ht="17" x14ac:dyDescent="0.2">
-      <c r="C15" t="s">
-        <v>78</v>
-      </c>
-      <c r="F15" t="s">
-        <v>74</v>
-      </c>
-      <c r="G15">
-        <v>1</v>
-      </c>
-      <c r="H15" s="1" t="s">
-        <v>76</v>
-      </c>
+      <c r="H35" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="I35" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="J35" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="K35" s="8" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A36" s="7"/>
+      <c r="B36" s="8"/>
+      <c r="C36" s="8"/>
+      <c r="D36" s="8"/>
+      <c r="E36" s="8"/>
+      <c r="F36" s="8"/>
+      <c r="G36" s="11"/>
+      <c r="H36" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="I36" s="8"/>
+      <c r="J36" s="8"/>
+      <c r="K36" s="8"/>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A37" s="7"/>
+      <c r="B37" s="8"/>
+      <c r="C37" s="8"/>
+      <c r="D37" s="8"/>
+      <c r="E37" s="8"/>
+      <c r="F37" s="8"/>
+      <c r="G37" s="11"/>
+      <c r="H37" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="I37" s="8"/>
+      <c r="J37" s="8"/>
+      <c r="K37" s="8"/>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A38" s="7"/>
+      <c r="B38" s="8"/>
+      <c r="C38" s="8"/>
+      <c r="D38" s="8"/>
+      <c r="E38" s="8"/>
+      <c r="F38" s="8"/>
+      <c r="G38" s="11"/>
+      <c r="H38" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="I38" s="8"/>
+      <c r="J38" s="8"/>
+      <c r="K38" s="8"/>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A39" s="7"/>
+      <c r="B39" s="8"/>
+      <c r="C39" s="8"/>
+      <c r="D39" s="8"/>
+      <c r="E39" s="8"/>
+      <c r="F39" s="8"/>
+      <c r="G39" s="11"/>
+      <c r="H39" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="I39" s="8"/>
+      <c r="J39" s="8"/>
+      <c r="K39" s="8"/>
     </row>
   </sheetData>
+  <mergeCells count="50">
+    <mergeCell ref="G35:G39"/>
+    <mergeCell ref="I35:I39"/>
+    <mergeCell ref="J35:J39"/>
+    <mergeCell ref="K35:K39"/>
+    <mergeCell ref="G31:G34"/>
+    <mergeCell ref="I31:I34"/>
+    <mergeCell ref="J31:J34"/>
+    <mergeCell ref="K31:K34"/>
+    <mergeCell ref="A35:A39"/>
+    <mergeCell ref="B35:B39"/>
+    <mergeCell ref="C35:C39"/>
+    <mergeCell ref="D35:D39"/>
+    <mergeCell ref="E35:E39"/>
+    <mergeCell ref="F35:F39"/>
+    <mergeCell ref="G27:G30"/>
+    <mergeCell ref="I27:I30"/>
+    <mergeCell ref="J27:J30"/>
+    <mergeCell ref="K27:K30"/>
+    <mergeCell ref="A31:A34"/>
+    <mergeCell ref="B31:B34"/>
+    <mergeCell ref="C31:C34"/>
+    <mergeCell ref="D31:D34"/>
+    <mergeCell ref="E31:E34"/>
+    <mergeCell ref="F31:F34"/>
+    <mergeCell ref="G23:G26"/>
+    <mergeCell ref="I23:I26"/>
+    <mergeCell ref="J23:J26"/>
+    <mergeCell ref="K23:K26"/>
+    <mergeCell ref="A27:A30"/>
+    <mergeCell ref="B27:B30"/>
+    <mergeCell ref="C27:C30"/>
+    <mergeCell ref="D27:D30"/>
+    <mergeCell ref="E27:E30"/>
+    <mergeCell ref="F27:F30"/>
+    <mergeCell ref="G19:G22"/>
+    <mergeCell ref="I19:I22"/>
+    <mergeCell ref="J19:J22"/>
+    <mergeCell ref="K19:K22"/>
+    <mergeCell ref="A23:A26"/>
+    <mergeCell ref="B23:B26"/>
+    <mergeCell ref="C23:C26"/>
+    <mergeCell ref="D23:D26"/>
+    <mergeCell ref="E23:E26"/>
+    <mergeCell ref="F23:F26"/>
+    <mergeCell ref="A19:A22"/>
+    <mergeCell ref="B19:B22"/>
+    <mergeCell ref="C19:C22"/>
+    <mergeCell ref="D19:D22"/>
+    <mergeCell ref="E19:E22"/>
+    <mergeCell ref="F19:F22"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Replace CSV mapping files Remove repeated symbol and change width for obliques to 2
</commit_message>
<xml_diff>
--- a/resources/4_mei_encoding/SQUAREnotation-NClevel.xlsx
+++ b/resources/4_mei_encoding/SQUAREnotation-NClevel.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mthomae/Documents/POSTDOC/ECHOES Project/2 OMR Part/1.0 Clean the layers &amp; update other resources/ic/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mthomae/Downloads/OMR_Portuguese_Sources/resources/4_mei_encoding/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09E589FE-4A8E-BC4C-8F89-D1C931CB8B88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{559AB2EF-7AD2-6948-BC24-CD4C758CDF1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="10760" yWindow="7960" windowWidth="38220" windowHeight="17440" xr2:uid="{C592A449-FCA0-F446-94A9-8EE74258CB16}"/>
   </bookViews>
@@ -165,7 +165,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="112">
   <si>
     <t>imagePath</t>
   </si>
@@ -1552,10 +1552,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7FC82D83-23D5-EB47-B9BB-AA65280E3DDF}">
-  <dimension ref="A1:K25"/>
+  <dimension ref="A1:K24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1730,7 +1730,7 @@
         <v>33</v>
       </c>
       <c r="G5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H5" s="1" t="s">
         <v>34</v>
@@ -1765,7 +1765,7 @@
         <v>38</v>
       </c>
       <c r="G6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H6" s="1" t="s">
         <v>39</v>
@@ -1800,7 +1800,7 @@
         <v>43</v>
       </c>
       <c r="G7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H7" s="1" t="s">
         <v>44</v>
@@ -2200,7 +2200,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:11" ht="102" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:11" ht="68" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>17</v>
       </c>
@@ -2235,7 +2235,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="1:11" ht="85" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:11" ht="68" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>17</v>
       </c>
@@ -2270,7 +2270,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="21" spans="1:11" ht="153" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:11" ht="68" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>17</v>
       </c>
@@ -2278,7 +2278,7 @@
         <v>17</v>
       </c>
       <c r="C21" t="s">
-        <v>31</v>
+        <v>100</v>
       </c>
       <c r="D21" t="s">
         <v>17</v>
@@ -2287,13 +2287,13 @@
         <v>17</v>
       </c>
       <c r="F21" t="s">
-        <v>33</v>
+        <v>101</v>
       </c>
       <c r="G21">
         <v>1</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>34</v>
+        <v>102</v>
       </c>
       <c r="I21" t="s">
         <v>17</v>
@@ -2305,7 +2305,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="22" spans="1:11" ht="119" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:11" ht="85" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>17</v>
       </c>
@@ -2313,7 +2313,7 @@
         <v>17</v>
       </c>
       <c r="C22" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="D22" t="s">
         <v>17</v>
@@ -2322,13 +2322,13 @@
         <v>17</v>
       </c>
       <c r="F22" t="s">
-        <v>101</v>
-      </c>
-      <c r="G22">
-        <v>1</v>
+        <v>104</v>
+      </c>
+      <c r="G22" t="s">
+        <v>65</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="I22" t="s">
         <v>17</v>
@@ -2340,7 +2340,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="23" spans="1:11" ht="136" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:11" ht="85" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>17</v>
       </c>
@@ -2348,7 +2348,7 @@
         <v>17</v>
       </c>
       <c r="C23" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="D23" t="s">
         <v>17</v>
@@ -2357,13 +2357,13 @@
         <v>17</v>
       </c>
       <c r="F23" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="G23" t="s">
         <v>65</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="I23" t="s">
         <v>17</v>
@@ -2375,7 +2375,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="24" spans="1:11" ht="136" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:11" ht="85" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>17</v>
       </c>
@@ -2383,7 +2383,7 @@
         <v>17</v>
       </c>
       <c r="C24" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="D24" t="s">
         <v>17</v>
@@ -2392,13 +2392,13 @@
         <v>17</v>
       </c>
       <c r="F24" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="G24" t="s">
         <v>65</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="I24" t="s">
         <v>17</v>
@@ -2407,41 +2407,6 @@
         <v>17</v>
       </c>
       <c r="K24" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11" ht="136" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
-        <v>17</v>
-      </c>
-      <c r="B25" t="s">
-        <v>17</v>
-      </c>
-      <c r="C25" t="s">
-        <v>109</v>
-      </c>
-      <c r="D25" t="s">
-        <v>17</v>
-      </c>
-      <c r="E25" t="s">
-        <v>17</v>
-      </c>
-      <c r="F25" t="s">
-        <v>110</v>
-      </c>
-      <c r="G25" t="s">
-        <v>65</v>
-      </c>
-      <c r="H25" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="I25" t="s">
-        <v>17</v>
-      </c>
-      <c r="J25" t="s">
-        <v>17</v>
-      </c>
-      <c r="K25" t="s">
         <v>17</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fix repeated notes (twolegsdown and lenguetaup) width
</commit_message>
<xml_diff>
--- a/resources/4_mei_encoding/SQUAREnotation-NClevel.xlsx
+++ b/resources/4_mei_encoding/SQUAREnotation-NClevel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mthomae/Downloads/OMR_Portuguese_Sources/resources/4_mei_encoding/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{559AB2EF-7AD2-6948-BC24-CD4C758CDF1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{313C0F27-FC79-934E-AD65-CB10CF91142D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="10760" yWindow="7960" windowWidth="38220" windowHeight="17440" xr2:uid="{C592A449-FCA0-F446-94A9-8EE74258CB16}"/>
   </bookViews>
@@ -165,7 +165,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="112">
   <si>
     <t>imagePath</t>
   </si>
@@ -1554,8 +1554,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7FC82D83-23D5-EB47-B9BB-AA65280E3DDF}">
   <dimension ref="A1:K24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H22" sqref="H22"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1904,8 +1904,8 @@
       <c r="F10" t="s">
         <v>59</v>
       </c>
-      <c r="G10">
-        <v>1</v>
+      <c r="G10" t="s">
+        <v>95</v>
       </c>
       <c r="H10" s="1" t="s">
         <v>60</v>
@@ -2289,8 +2289,8 @@
       <c r="F21" t="s">
         <v>101</v>
       </c>
-      <c r="G21">
-        <v>1</v>
+      <c r="G21" t="s">
+        <v>95</v>
       </c>
       <c r="H21" s="1" t="s">
         <v>102</v>

</xml_diff>

<commit_message>
Fix 'type' dissapearing for repeated notes The fix was to move the '@type = twolegsdown' and '@type = lenguetaup' to the 'nc' instead of the 'neume' as it gets lost in 'neume' when this is combined with others (forming a larger neume) in the MEI Encoding job. We would need a postprocessing step to change every two consecutive 'nc' with 'type=twolegsdown' or 'type=lenguetaup' (or 'twolegsup' or 'lenguetadown') into 'neume' with that type (after Neon correction).
</commit_message>
<xml_diff>
--- a/resources/4_mei_encoding/SQUAREnotation-NClevel.xlsx
+++ b/resources/4_mei_encoding/SQUAREnotation-NClevel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mthomae/Downloads/OMR_Portuguese_Sources/resources/4_mei_encoding/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{313C0F27-FC79-934E-AD65-CB10CF91142D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B497F2D6-34FC-9841-B151-A2D342D09C45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="10760" yWindow="7960" windowWidth="38220" windowHeight="17440" xr2:uid="{C592A449-FCA0-F446-94A9-8EE74258CB16}"/>
   </bookViews>
@@ -368,12 +368,6 @@
     <t>neume.lenguetaup</t>
   </si>
   <si>
-    <t>&lt;neume type="lenguetaup"&gt;
-    &lt;nc/&gt;
-    &lt;nc intm="0S"/&gt;
-&lt;/neume&gt;</t>
-  </si>
-  <si>
     <t>https://pemdatabase.eu/iipsrv/iipsrv.fcgi?IIIF=images/cc7b84c3-df67-4556-91fb-2b9eb9e8b6bd/pk5Nfb9x14858.tiff/2626,1780,104,86/128,/0/default.jpg</t>
   </si>
   <si>
@@ -515,12 +509,6 @@
     <t>neume.twolegsdown</t>
   </si>
   <si>
-    <t>&lt;neume type="twolegsdown"&gt;
-    &lt;nc/&gt;
-    &lt;nc intm="0S"/&gt;
-&lt;/neume&gt;</t>
-  </si>
-  <si>
     <t>Torculus11</t>
   </si>
   <si>
@@ -557,6 +545,18 @@
     &lt;nc/&gt;
     &lt;nc intm="1S"/&gt;
     &lt;nc intm="-3S"/&gt;
+&lt;/neume&gt;</t>
+  </si>
+  <si>
+    <t>&lt;neume&gt;
+    &lt;nc type="lenguetaup"/&gt;
+    &lt;nc intm="0S" type="lenguetaup"/&gt;
+&lt;/neume&gt;</t>
+  </si>
+  <si>
+    <t>&lt;neume&gt;
+    &lt;nc type="twolegsdown"/&gt;
+    &lt;nc intm="0S" type="twolegsdown"/&gt;
 &lt;/neume&gt;</t>
   </si>
 </sst>
@@ -1554,8 +1554,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7FC82D83-23D5-EB47-B9BB-AA65280E3DDF}">
   <dimension ref="A1:K24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1566,7 +1566,7 @@
     <col min="4" max="4" width="4.6640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="32" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="19.83203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="31.6640625" customWidth="1"/>
+    <col min="8" max="8" width="39" customWidth="1"/>
     <col min="11" max="11" width="12.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1905,10 +1905,10 @@
         <v>59</v>
       </c>
       <c r="G10" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>60</v>
+        <v>110</v>
       </c>
       <c r="I10" t="s">
         <v>17</v>
@@ -1922,28 +1922,28 @@
     </row>
     <row r="11" spans="1:11" ht="85" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B11" t="e" vm="10">
         <v>#VALUE!</v>
       </c>
       <c r="C11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D11">
         <v>91</v>
       </c>
       <c r="E11" t="s">
+        <v>62</v>
+      </c>
+      <c r="F11" t="s">
         <v>63</v>
       </c>
-      <c r="F11" t="s">
+      <c r="G11" t="s">
         <v>64</v>
       </c>
-      <c r="G11" t="s">
+      <c r="H11" s="1" t="s">
         <v>65</v>
-      </c>
-      <c r="H11" s="1" t="s">
-        <v>66</v>
       </c>
       <c r="I11" t="s">
         <v>17</v>
@@ -1957,28 +1957,28 @@
     </row>
     <row r="12" spans="1:11" ht="85" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B12" t="e" vm="11">
         <v>#VALUE!</v>
       </c>
       <c r="C12" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D12">
         <v>12</v>
       </c>
       <c r="E12" t="s">
+        <v>68</v>
+      </c>
+      <c r="F12" t="s">
         <v>69</v>
       </c>
-      <c r="F12" t="s">
+      <c r="G12" t="s">
+        <v>64</v>
+      </c>
+      <c r="H12" s="1" t="s">
         <v>70</v>
-      </c>
-      <c r="G12" t="s">
-        <v>65</v>
-      </c>
-      <c r="H12" s="1" t="s">
-        <v>71</v>
       </c>
       <c r="I12" t="s">
         <v>17</v>
@@ -1992,37 +1992,37 @@
     </row>
     <row r="13" spans="1:11" ht="85" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B13" t="e" vm="12">
         <v>#VALUE!</v>
       </c>
       <c r="C13" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D13">
         <v>3</v>
       </c>
       <c r="E13" t="s">
+        <v>73</v>
+      </c>
+      <c r="F13" t="s">
         <v>74</v>
       </c>
-      <c r="F13" t="s">
+      <c r="G13" t="s">
+        <v>64</v>
+      </c>
+      <c r="H13" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="G13" t="s">
-        <v>65</v>
-      </c>
-      <c r="H13" s="1" t="s">
+      <c r="I13" t="s">
+        <v>17</v>
+      </c>
+      <c r="J13" t="s">
+        <v>17</v>
+      </c>
+      <c r="K13" t="s">
         <v>76</v>
-      </c>
-      <c r="I13" t="s">
-        <v>17</v>
-      </c>
-      <c r="J13" t="s">
-        <v>17</v>
-      </c>
-      <c r="K13" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.2">
@@ -2033,22 +2033,22 @@
         <v>17</v>
       </c>
       <c r="C14" t="s">
+        <v>77</v>
+      </c>
+      <c r="D14" t="s">
+        <v>17</v>
+      </c>
+      <c r="E14" t="s">
+        <v>17</v>
+      </c>
+      <c r="F14" t="s">
         <v>78</v>
-      </c>
-      <c r="D14" t="s">
-        <v>17</v>
-      </c>
-      <c r="E14" t="s">
-        <v>17</v>
-      </c>
-      <c r="F14" t="s">
-        <v>79</v>
       </c>
       <c r="G14">
         <v>1</v>
       </c>
       <c r="H14" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I14" t="s">
         <v>17</v>
@@ -2068,22 +2068,22 @@
         <v>17</v>
       </c>
       <c r="C15" t="s">
+        <v>80</v>
+      </c>
+      <c r="D15" t="s">
+        <v>17</v>
+      </c>
+      <c r="E15" t="s">
+        <v>17</v>
+      </c>
+      <c r="F15" t="s">
         <v>81</v>
-      </c>
-      <c r="D15" t="s">
-        <v>17</v>
-      </c>
-      <c r="E15" t="s">
-        <v>17</v>
-      </c>
-      <c r="F15" t="s">
-        <v>82</v>
       </c>
       <c r="G15">
         <v>1</v>
       </c>
       <c r="H15" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="I15" t="s">
         <v>17</v>
@@ -2103,22 +2103,22 @@
         <v>17</v>
       </c>
       <c r="C16" t="s">
+        <v>83</v>
+      </c>
+      <c r="D16" t="s">
+        <v>17</v>
+      </c>
+      <c r="E16" t="s">
+        <v>17</v>
+      </c>
+      <c r="F16" t="s">
         <v>84</v>
-      </c>
-      <c r="D16" t="s">
-        <v>17</v>
-      </c>
-      <c r="E16" t="s">
-        <v>17</v>
-      </c>
-      <c r="F16" t="s">
-        <v>85</v>
       </c>
       <c r="G16">
         <v>1</v>
       </c>
       <c r="H16" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="I16" t="s">
         <v>17</v>
@@ -2138,22 +2138,22 @@
         <v>17</v>
       </c>
       <c r="C17" t="s">
+        <v>86</v>
+      </c>
+      <c r="D17" t="s">
+        <v>17</v>
+      </c>
+      <c r="E17" t="s">
+        <v>17</v>
+      </c>
+      <c r="F17" t="s">
         <v>87</v>
-      </c>
-      <c r="D17" t="s">
-        <v>17</v>
-      </c>
-      <c r="E17" t="s">
-        <v>17</v>
-      </c>
-      <c r="F17" t="s">
-        <v>88</v>
       </c>
       <c r="G17">
         <v>1</v>
       </c>
       <c r="H17" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="I17" t="s">
         <v>17</v>
@@ -2173,22 +2173,22 @@
         <v>17</v>
       </c>
       <c r="C18" t="s">
+        <v>89</v>
+      </c>
+      <c r="D18" t="s">
+        <v>17</v>
+      </c>
+      <c r="E18" t="s">
+        <v>17</v>
+      </c>
+      <c r="F18" t="s">
         <v>90</v>
-      </c>
-      <c r="D18" t="s">
-        <v>17</v>
-      </c>
-      <c r="E18" t="s">
-        <v>17</v>
-      </c>
-      <c r="F18" t="s">
-        <v>91</v>
       </c>
       <c r="G18">
         <v>1</v>
       </c>
       <c r="H18" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="I18" t="s">
         <v>17</v>
@@ -2208,22 +2208,22 @@
         <v>17</v>
       </c>
       <c r="C19" t="s">
+        <v>92</v>
+      </c>
+      <c r="D19" t="s">
+        <v>17</v>
+      </c>
+      <c r="E19" t="s">
+        <v>17</v>
+      </c>
+      <c r="F19" t="s">
         <v>93</v>
       </c>
-      <c r="D19" t="s">
-        <v>17</v>
-      </c>
-      <c r="E19" t="s">
-        <v>17</v>
-      </c>
-      <c r="F19" t="s">
+      <c r="G19" t="s">
         <v>94</v>
       </c>
-      <c r="G19" t="s">
+      <c r="H19" s="1" t="s">
         <v>95</v>
-      </c>
-      <c r="H19" s="1" t="s">
-        <v>96</v>
       </c>
       <c r="I19" t="s">
         <v>17</v>
@@ -2243,57 +2243,57 @@
         <v>17</v>
       </c>
       <c r="C20" t="s">
+        <v>96</v>
+      </c>
+      <c r="D20" t="s">
+        <v>17</v>
+      </c>
+      <c r="E20" t="s">
+        <v>17</v>
+      </c>
+      <c r="F20" t="s">
         <v>97</v>
       </c>
-      <c r="D20" t="s">
-        <v>17</v>
-      </c>
-      <c r="E20" t="s">
-        <v>17</v>
-      </c>
-      <c r="F20" t="s">
+      <c r="G20" t="s">
+        <v>94</v>
+      </c>
+      <c r="H20" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="G20" t="s">
-        <v>95</v>
-      </c>
-      <c r="H20" s="1" t="s">
+      <c r="I20" t="s">
+        <v>17</v>
+      </c>
+      <c r="J20" t="s">
+        <v>17</v>
+      </c>
+      <c r="K20" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" ht="85" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>17</v>
+      </c>
+      <c r="B21" t="s">
+        <v>17</v>
+      </c>
+      <c r="C21" t="s">
         <v>99</v>
       </c>
-      <c r="I20" t="s">
-        <v>17</v>
-      </c>
-      <c r="J20" t="s">
-        <v>17</v>
-      </c>
-      <c r="K20" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" ht="68" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
-        <v>17</v>
-      </c>
-      <c r="B21" t="s">
-        <v>17</v>
-      </c>
-      <c r="C21" t="s">
+      <c r="D21" t="s">
+        <v>17</v>
+      </c>
+      <c r="E21" t="s">
+        <v>17</v>
+      </c>
+      <c r="F21" t="s">
         <v>100</v>
       </c>
-      <c r="D21" t="s">
-        <v>17</v>
-      </c>
-      <c r="E21" t="s">
-        <v>17</v>
-      </c>
-      <c r="F21" t="s">
-        <v>101</v>
-      </c>
       <c r="G21" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>102</v>
+        <v>111</v>
       </c>
       <c r="I21" t="s">
         <v>17</v>
@@ -2313,22 +2313,22 @@
         <v>17</v>
       </c>
       <c r="C22" t="s">
+        <v>101</v>
+      </c>
+      <c r="D22" t="s">
+        <v>17</v>
+      </c>
+      <c r="E22" t="s">
+        <v>17</v>
+      </c>
+      <c r="F22" t="s">
+        <v>102</v>
+      </c>
+      <c r="G22" t="s">
+        <v>64</v>
+      </c>
+      <c r="H22" s="1" t="s">
         <v>103</v>
-      </c>
-      <c r="D22" t="s">
-        <v>17</v>
-      </c>
-      <c r="E22" t="s">
-        <v>17</v>
-      </c>
-      <c r="F22" t="s">
-        <v>104</v>
-      </c>
-      <c r="G22" t="s">
-        <v>65</v>
-      </c>
-      <c r="H22" s="1" t="s">
-        <v>105</v>
       </c>
       <c r="I22" t="s">
         <v>17</v>
@@ -2348,22 +2348,22 @@
         <v>17</v>
       </c>
       <c r="C23" t="s">
+        <v>104</v>
+      </c>
+      <c r="D23" t="s">
+        <v>17</v>
+      </c>
+      <c r="E23" t="s">
+        <v>17</v>
+      </c>
+      <c r="F23" t="s">
+        <v>105</v>
+      </c>
+      <c r="G23" t="s">
+        <v>64</v>
+      </c>
+      <c r="H23" s="1" t="s">
         <v>106</v>
-      </c>
-      <c r="D23" t="s">
-        <v>17</v>
-      </c>
-      <c r="E23" t="s">
-        <v>17</v>
-      </c>
-      <c r="F23" t="s">
-        <v>107</v>
-      </c>
-      <c r="G23" t="s">
-        <v>65</v>
-      </c>
-      <c r="H23" s="1" t="s">
-        <v>108</v>
       </c>
       <c r="I23" t="s">
         <v>17</v>
@@ -2383,22 +2383,22 @@
         <v>17</v>
       </c>
       <c r="C24" t="s">
+        <v>107</v>
+      </c>
+      <c r="D24" t="s">
+        <v>17</v>
+      </c>
+      <c r="E24" t="s">
+        <v>17</v>
+      </c>
+      <c r="F24" t="s">
+        <v>108</v>
+      </c>
+      <c r="G24" t="s">
+        <v>64</v>
+      </c>
+      <c r="H24" s="1" t="s">
         <v>109</v>
-      </c>
-      <c r="D24" t="s">
-        <v>17</v>
-      </c>
-      <c r="E24" t="s">
-        <v>17</v>
-      </c>
-      <c r="F24" t="s">
-        <v>110</v>
-      </c>
-      <c r="G24" t="s">
-        <v>65</v>
-      </c>
-      <c r="H24" s="1" t="s">
-        <v>111</v>
       </c>
       <c r="I24" t="s">
         <v>17</v>

</xml_diff>